<commit_message>
All things wishlist have been added and correctly work
</commit_message>
<xml_diff>
--- a/jasonH-wsp21-ProductSprintBackLog.xlsx
+++ b/jasonH-wsp21-ProductSprintBackLog.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="98">
   <si>
     <t>Category</t>
   </si>
@@ -297,9 +297,6 @@
     <t>Sprint Backlog: Sprint 2</t>
   </si>
   <si>
-    <t>When viewing a product there is a comment button</t>
-  </si>
-  <si>
     <t>&lt;As a&gt; user, &lt;I want to&gt; have a way to view comments/reviews</t>
   </si>
   <si>
@@ -350,12 +347,18 @@
   <si>
     <t>On the comment page there is a place comment button</t>
   </si>
+  <si>
+    <t>When viewing a product as a user there is a comment button</t>
+  </si>
+  <si>
+    <t>Guest can view comments before signing in</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -464,6 +467,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -491,7 +500,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="62">
+  <borders count="78">
     <border>
       <left/>
       <right/>
@@ -1284,11 +1293,221 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="184">
+  <cellXfs count="198">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1598,9 +1817,6 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1608,25 +1824,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1734,14 +1938,69 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2098,10 +2357,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="153" t="s">
+      <c r="A2" s="148" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="155" t="s">
+      <c r="B2" s="150" t="s">
         <v>47</v>
       </c>
       <c r="C2" s="56">
@@ -2115,8 +2374,8 @@
       <c r="G2" s="58"/>
     </row>
     <row r="3" spans="1:7" s="89" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="154"/>
-      <c r="B3" s="156"/>
+      <c r="A3" s="149"/>
+      <c r="B3" s="151"/>
       <c r="C3" s="84">
         <v>2</v>
       </c>
@@ -2128,8 +2387,8 @@
       <c r="G3" s="86"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="154"/>
-      <c r="B4" s="156"/>
+      <c r="A4" s="149"/>
+      <c r="B4" s="151"/>
       <c r="C4" s="84">
         <v>3</v>
       </c>
@@ -2141,8 +2400,8 @@
       <c r="G4" s="86"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="154"/>
-      <c r="B5" s="156" t="s">
+      <c r="A5" s="149"/>
+      <c r="B5" s="151" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="84">
@@ -2156,8 +2415,8 @@
       <c r="G5" s="86"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="154"/>
-      <c r="B6" s="156"/>
+      <c r="A6" s="149"/>
+      <c r="B6" s="151"/>
       <c r="C6" s="84">
         <v>5</v>
       </c>
@@ -2169,8 +2428,8 @@
       <c r="G6" s="86"/>
     </row>
     <row r="7" spans="1:7" s="90" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="154"/>
-      <c r="B7" s="156"/>
+      <c r="A7" s="149"/>
+      <c r="B7" s="151"/>
       <c r="C7" s="84">
         <v>6</v>
       </c>
@@ -2182,8 +2441,8 @@
       <c r="G7" s="86"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="154"/>
-      <c r="B8" s="157" t="s">
+      <c r="A8" s="149"/>
+      <c r="B8" s="152" t="s">
         <v>38</v>
       </c>
       <c r="C8" s="84">
@@ -2197,8 +2456,8 @@
       <c r="G8" s="86"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="154"/>
-      <c r="B9" s="157"/>
+      <c r="A9" s="149"/>
+      <c r="B9" s="152"/>
       <c r="C9" s="84">
         <v>8</v>
       </c>
@@ -2210,8 +2469,8 @@
       <c r="G9" s="86"/>
     </row>
     <row r="10" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="154"/>
-      <c r="B10" s="157"/>
+      <c r="A10" s="149"/>
+      <c r="B10" s="152"/>
       <c r="C10" s="84">
         <v>9</v>
       </c>
@@ -2223,7 +2482,7 @@
       <c r="G10" s="86"/>
     </row>
     <row r="11" spans="1:7" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="154"/>
+      <c r="A11" s="149"/>
       <c r="B11" s="114"/>
       <c r="C11" s="84">
         <v>10</v>
@@ -2236,7 +2495,7 @@
       <c r="G11" s="86"/>
     </row>
     <row r="12" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="154"/>
+      <c r="A12" s="149"/>
       <c r="B12" s="114"/>
       <c r="C12" s="84">
         <v>11</v>
@@ -2249,7 +2508,7 @@
       <c r="G12" s="86"/>
     </row>
     <row r="13" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="154"/>
+      <c r="A13" s="149"/>
       <c r="B13" s="102"/>
       <c r="C13" s="53">
         <v>12</v>
@@ -2263,7 +2522,7 @@
     </row>
     <row r="14" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="110"/>
-      <c r="B14" s="158" t="s">
+      <c r="B14" s="153" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="111">
@@ -2277,10 +2536,10 @@
       <c r="G14" s="62"/>
     </row>
     <row r="15" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="161" t="s">
+      <c r="A15" s="156" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="159"/>
+      <c r="B15" s="154"/>
       <c r="C15" s="59">
         <v>14</v>
       </c>
@@ -2292,8 +2551,8 @@
       <c r="G15" s="61"/>
     </row>
     <row r="16" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="162"/>
-      <c r="B16" s="159"/>
+      <c r="A16" s="157"/>
+      <c r="B16" s="154"/>
       <c r="C16" s="91">
         <v>15</v>
       </c>
@@ -2305,8 +2564,8 @@
       <c r="G16" s="93"/>
     </row>
     <row r="17" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="162"/>
-      <c r="B17" s="159"/>
+      <c r="A17" s="157"/>
+      <c r="B17" s="154"/>
       <c r="C17" s="91">
         <v>16</v>
       </c>
@@ -2318,8 +2577,8 @@
       <c r="G17" s="93"/>
     </row>
     <row r="18" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="162"/>
-      <c r="B18" s="160"/>
+      <c r="A18" s="157"/>
+      <c r="B18" s="155"/>
       <c r="C18" s="63">
         <v>17</v>
       </c>
@@ -2331,8 +2590,8 @@
       <c r="G18" s="65"/>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="162"/>
-      <c r="B19" s="164" t="s">
+      <c r="A19" s="157"/>
+      <c r="B19" s="159" t="s">
         <v>35</v>
       </c>
       <c r="C19" s="98">
@@ -2346,8 +2605,8 @@
       <c r="G19" s="101"/>
     </row>
     <row r="20" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="162"/>
-      <c r="B20" s="164"/>
+      <c r="A20" s="157"/>
+      <c r="B20" s="159"/>
       <c r="C20" s="98">
         <v>19</v>
       </c>
@@ -2359,8 +2618,8 @@
       <c r="G20" s="101"/>
     </row>
     <row r="21" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="163"/>
-      <c r="B21" s="165"/>
+      <c r="A21" s="158"/>
+      <c r="B21" s="160"/>
       <c r="C21" s="106">
         <v>20</v>
       </c>
@@ -2372,8 +2631,8 @@
       <c r="G21" s="109"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="149"/>
-      <c r="B22" s="151"/>
+      <c r="A22" s="144"/>
+      <c r="B22" s="146"/>
       <c r="C22" s="66"/>
       <c r="D22" s="67"/>
       <c r="E22" s="67"/>
@@ -2381,8 +2640,8 @@
       <c r="G22" s="69"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="150"/>
-      <c r="B23" s="152"/>
+      <c r="A23" s="145"/>
+      <c r="B23" s="147"/>
       <c r="C23" s="70"/>
       <c r="D23" s="71"/>
       <c r="E23" s="72"/>
@@ -2424,12 +2683,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" s="24" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="183" t="s">
+      <c r="A3" s="176" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="183"/>
-      <c r="C3" s="183"/>
-      <c r="D3" s="183"/>
+      <c r="B3" s="176"/>
+      <c r="C3" s="176"/>
+      <c r="D3" s="176"/>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:4" s="27" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2543,16 +2802,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="166" t="s">
+      <c r="A1" s="161" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
+      <c r="B1" s="161"/>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="161"/>
+      <c r="G1" s="161"/>
+      <c r="H1" s="161"/>
       <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -2592,7 +2851,7 @@
       <c r="I3" s="10"/>
     </row>
     <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="153" t="s">
+      <c r="A4" s="148" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="116"/>
@@ -2605,7 +2864,7 @@
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="154"/>
+      <c r="A5" s="149"/>
       <c r="B5" s="102"/>
       <c r="C5" s="84">
         <v>1</v>
@@ -2620,7 +2879,7 @@
       <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="154"/>
+      <c r="A6" s="149"/>
       <c r="B6" s="102"/>
       <c r="C6" s="84"/>
       <c r="D6" s="54"/>
@@ -2631,7 +2890,7 @@
       <c r="I6" s="9"/>
     </row>
     <row r="7" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="154"/>
+      <c r="A7" s="149"/>
       <c r="B7" s="102"/>
       <c r="C7" s="84"/>
       <c r="D7" s="16"/>
@@ -2642,7 +2901,7 @@
       <c r="I7" s="9"/>
     </row>
     <row r="8" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="154"/>
+      <c r="A8" s="149"/>
       <c r="B8" s="102"/>
       <c r="C8" s="84"/>
       <c r="D8" s="104"/>
@@ -2653,7 +2912,7 @@
       <c r="I8" s="9"/>
     </row>
     <row r="9" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="154"/>
+      <c r="A9" s="149"/>
       <c r="B9" s="102"/>
       <c r="C9" s="84"/>
       <c r="D9" s="16"/>
@@ -2664,7 +2923,7 @@
       <c r="I9" s="9"/>
     </row>
     <row r="10" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="154"/>
+      <c r="A10" s="149"/>
       <c r="B10" s="102"/>
       <c r="C10" s="84"/>
       <c r="D10" s="16"/>
@@ -2675,7 +2934,7 @@
       <c r="I10" s="9"/>
     </row>
     <row r="11" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="154"/>
+      <c r="A11" s="149"/>
       <c r="B11" s="102"/>
       <c r="C11" s="84"/>
       <c r="D11" s="16"/>
@@ -2686,7 +2945,7 @@
       <c r="I11" s="9"/>
     </row>
     <row r="12" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="154"/>
+      <c r="A12" s="149"/>
       <c r="B12" s="102"/>
       <c r="C12" s="84"/>
       <c r="D12" s="16"/>
@@ -2697,7 +2956,7 @@
       <c r="I12" s="9"/>
     </row>
     <row r="13" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="154"/>
+      <c r="A13" s="149"/>
       <c r="B13" s="103"/>
       <c r="C13" s="84"/>
       <c r="D13" s="16"/>
@@ -2708,7 +2967,7 @@
       <c r="I13" s="9"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="154"/>
+      <c r="A14" s="149"/>
       <c r="B14" s="103"/>
       <c r="C14" s="84"/>
       <c r="D14" s="16"/>
@@ -2719,7 +2978,7 @@
       <c r="I14" s="9"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="154"/>
+      <c r="A15" s="149"/>
       <c r="B15" s="102"/>
       <c r="C15" s="53"/>
       <c r="D15" s="16"/>
@@ -2729,10 +2988,10 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="170" t="s">
+      <c r="A16" s="165" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="164" t="s">
+      <c r="B16" s="159" t="s">
         <v>35</v>
       </c>
       <c r="C16" s="111">
@@ -2747,8 +3006,8 @@
       <c r="H16" s="16"/>
     </row>
     <row r="17" spans="1:9" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="154"/>
-      <c r="B17" s="164"/>
+      <c r="A17" s="149"/>
+      <c r="B17" s="159"/>
       <c r="C17" s="59">
         <v>3</v>
       </c>
@@ -2762,8 +3021,8 @@
       <c r="I17" s="9"/>
     </row>
     <row r="18" spans="1:9" ht="26.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="154"/>
-      <c r="B18" s="165"/>
+      <c r="A18" s="149"/>
+      <c r="B18" s="160"/>
       <c r="C18" s="91">
         <v>4</v>
       </c>
@@ -2777,8 +3036,8 @@
       <c r="I18" s="9"/>
     </row>
     <row r="19" spans="1:9" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="154"/>
-      <c r="B19" s="158" t="s">
+      <c r="A19" s="149"/>
+      <c r="B19" s="153" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="91">
@@ -2794,8 +3053,8 @@
       <c r="I19" s="9"/>
     </row>
     <row r="20" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="154"/>
-      <c r="B20" s="159"/>
+      <c r="A20" s="149"/>
+      <c r="B20" s="154"/>
       <c r="C20" s="63">
         <v>6</v>
       </c>
@@ -2807,8 +3066,8 @@
       <c r="G20" s="65"/>
     </row>
     <row r="21" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="154"/>
-      <c r="B21" s="159"/>
+      <c r="A21" s="149"/>
+      <c r="B21" s="154"/>
       <c r="C21" s="98">
         <v>7</v>
       </c>
@@ -2820,8 +3079,8 @@
       <c r="G21" s="101"/>
     </row>
     <row r="22" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="154"/>
-      <c r="B22" s="159"/>
+      <c r="A22" s="149"/>
+      <c r="B22" s="154"/>
       <c r="C22" s="98"/>
       <c r="D22" s="64"/>
       <c r="E22" s="99"/>
@@ -2829,8 +3088,8 @@
       <c r="G22" s="101"/>
     </row>
     <row r="23" spans="1:9" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="171"/>
-      <c r="B23" s="160"/>
+      <c r="A23" s="166"/>
+      <c r="B23" s="155"/>
       <c r="C23" s="106"/>
       <c r="D23" s="105"/>
       <c r="E23" s="107"/>
@@ -2838,8 +3097,8 @@
       <c r="G23" s="109"/>
     </row>
     <row r="24" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="149"/>
-      <c r="B24" s="151"/>
+      <c r="A24" s="144"/>
+      <c r="B24" s="146"/>
       <c r="C24" s="66"/>
       <c r="D24" s="67"/>
       <c r="E24" s="67"/>
@@ -2847,8 +3106,8 @@
       <c r="G24" s="69"/>
     </row>
     <row r="25" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="150"/>
-      <c r="B25" s="152"/>
+      <c r="A25" s="145"/>
+      <c r="B25" s="147"/>
       <c r="C25" s="70"/>
       <c r="D25" s="71"/>
       <c r="E25" s="72"/>
@@ -2856,38 +3115,38 @@
       <c r="G25" s="73"/>
     </row>
     <row r="26" spans="1:9" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="168" t="s">
+      <c r="A26" s="163" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="168"/>
-      <c r="C26" s="168"/>
-      <c r="D26" s="168"/>
+      <c r="B26" s="163"/>
+      <c r="C26" s="163"/>
+      <c r="D26" s="163"/>
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
       <c r="G26" s="18"/>
       <c r="H26" s="17"/>
     </row>
     <row r="27" spans="1:9" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="169" t="s">
+      <c r="A27" s="164" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="169"/>
-      <c r="C27" s="169"/>
-      <c r="D27" s="169"/>
-      <c r="E27" s="169"/>
-      <c r="F27" s="169"/>
-      <c r="G27" s="169"/>
+      <c r="B27" s="164"/>
+      <c r="C27" s="164"/>
+      <c r="D27" s="164"/>
+      <c r="E27" s="164"/>
+      <c r="F27" s="164"/>
+      <c r="G27" s="164"/>
       <c r="H27" s="20"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="167" t="s">
+      <c r="A28" s="162" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="167"/>
-      <c r="C28" s="167"/>
-      <c r="D28" s="167"/>
-      <c r="E28" s="167"/>
-      <c r="F28" s="167"/>
+      <c r="B28" s="162"/>
+      <c r="C28" s="162"/>
+      <c r="D28" s="162"/>
+      <c r="E28" s="162"/>
+      <c r="F28" s="162"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2950,7 +3209,7 @@
       </c>
     </row>
     <row r="3" spans="1:1026" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="175"/>
+      <c r="A3" s="170"/>
       <c r="B3" s="29"/>
       <c r="C3" s="39"/>
       <c r="D3" s="39"/>
@@ -2959,7 +3218,7 @@
       <c r="G3" s="32"/>
     </row>
     <row r="4" spans="1:1026" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="175"/>
+      <c r="A4" s="170"/>
       <c r="B4" s="30"/>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
@@ -2968,7 +3227,7 @@
       <c r="G4" s="33"/>
     </row>
     <row r="5" spans="1:1026" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="175"/>
+      <c r="A5" s="170"/>
       <c r="B5" s="96"/>
       <c r="C5" s="39"/>
       <c r="D5" s="39"/>
@@ -2977,7 +3236,7 @@
       <c r="G5" s="33"/>
     </row>
     <row r="6" spans="1:1026" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="175"/>
+      <c r="A6" s="170"/>
       <c r="B6" s="96"/>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
@@ -2986,7 +3245,7 @@
       <c r="G6" s="33"/>
     </row>
     <row r="7" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="175"/>
+      <c r="A7" s="170"/>
       <c r="B7" s="31"/>
       <c r="C7" s="39"/>
       <c r="D7" s="39"/>
@@ -2995,7 +3254,7 @@
       <c r="G7" s="34"/>
     </row>
     <row r="8" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="175"/>
+      <c r="A8" s="170"/>
       <c r="B8" s="97"/>
       <c r="C8" s="39"/>
       <c r="D8" s="39"/>
@@ -3004,7 +3263,7 @@
       <c r="G8" s="35"/>
     </row>
     <row r="9" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="175">
+      <c r="A9" s="170">
         <v>1</v>
       </c>
       <c r="B9" s="120" t="s">
@@ -3025,7 +3284,7 @@
       <c r="G9" s="36"/>
     </row>
     <row r="10" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="175"/>
+      <c r="A10" s="170"/>
       <c r="B10" s="30" t="s">
         <v>65</v>
       </c>
@@ -3044,7 +3303,7 @@
       <c r="G10" s="37"/>
     </row>
     <row r="11" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="175"/>
+      <c r="A11" s="170"/>
       <c r="B11" s="30" t="s">
         <v>67</v>
       </c>
@@ -3063,7 +3322,7 @@
       <c r="G11" s="37"/>
     </row>
     <row r="12" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="175"/>
+      <c r="A12" s="170"/>
       <c r="B12" s="21" t="s">
         <v>77</v>
       </c>
@@ -3082,7 +3341,7 @@
       <c r="G12" s="37"/>
     </row>
     <row r="13" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="175"/>
+      <c r="A13" s="170"/>
       <c r="B13" s="30" t="s">
         <v>66</v>
       </c>
@@ -3101,7 +3360,7 @@
       <c r="G13" s="35"/>
     </row>
     <row r="14" spans="1:1026" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="175">
+      <c r="A14" s="170">
         <v>2</v>
       </c>
       <c r="B14" s="29" t="s">
@@ -3122,7 +3381,7 @@
       <c r="G14" s="32"/>
     </row>
     <row r="15" spans="1:1026" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="175"/>
+      <c r="A15" s="170"/>
       <c r="B15" s="117" t="s">
         <v>60</v>
       </c>
@@ -4160,7 +4419,7 @@
       <c r="AML15" s="115"/>
     </row>
     <row r="16" spans="1:1026" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="175"/>
+      <c r="A16" s="170"/>
       <c r="B16" s="117" t="s">
         <v>61</v>
       </c>
@@ -5198,7 +5457,7 @@
       <c r="AML16" s="115"/>
     </row>
     <row r="17" spans="1:1026" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="175"/>
+      <c r="A17" s="170"/>
       <c r="B17" s="117" t="s">
         <v>63</v>
       </c>
@@ -6236,7 +6495,7 @@
       <c r="AML17" s="115"/>
     </row>
     <row r="18" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="175"/>
+      <c r="A18" s="170"/>
       <c r="B18" s="96" t="s">
         <v>64</v>
       </c>
@@ -6255,7 +6514,7 @@
       <c r="G18" s="37"/>
     </row>
     <row r="19" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="172">
+      <c r="A19" s="167">
         <v>3</v>
       </c>
       <c r="B19" s="74" t="s">
@@ -7295,7 +7554,7 @@
       <c r="AML19" s="81"/>
     </row>
     <row r="20" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="173"/>
+      <c r="A20" s="168"/>
       <c r="B20" s="75" t="s">
         <v>69</v>
       </c>
@@ -8333,7 +8592,7 @@
       <c r="AML20" s="81"/>
     </row>
     <row r="21" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="173"/>
+      <c r="A21" s="168"/>
       <c r="B21" s="75" t="s">
         <v>70</v>
       </c>
@@ -9371,7 +9630,7 @@
       <c r="AML21" s="81"/>
     </row>
     <row r="22" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="172">
+      <c r="A22" s="167">
         <v>4</v>
       </c>
       <c r="B22" s="74" t="s">
@@ -10411,7 +10670,7 @@
       <c r="AML22" s="81"/>
     </row>
     <row r="23" spans="1:1026" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="173"/>
+      <c r="A23" s="168"/>
       <c r="B23" s="75" t="s">
         <v>72</v>
       </c>
@@ -11449,7 +11708,7 @@
       <c r="AML23" s="81"/>
     </row>
     <row r="24" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="173"/>
+      <c r="A24" s="168"/>
       <c r="B24" s="75" t="s">
         <v>73</v>
       </c>
@@ -12487,7 +12746,7 @@
       <c r="AML24" s="81"/>
     </row>
     <row r="25" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="173"/>
+      <c r="A25" s="168"/>
       <c r="B25" s="75" t="s">
         <v>74</v>
       </c>
@@ -13525,7 +13784,7 @@
       <c r="AML25" s="81"/>
     </row>
     <row r="26" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="174"/>
+      <c r="A26" s="169"/>
       <c r="B26" s="76" t="s">
         <v>75</v>
       </c>
@@ -14563,7 +14822,7 @@
       <c r="AML26" s="81"/>
     </row>
     <row r="27" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="172">
+      <c r="A27" s="167">
         <v>5</v>
       </c>
       <c r="B27" s="74" t="s">
@@ -15603,7 +15862,7 @@
       <c r="AML27" s="81"/>
     </row>
     <row r="28" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="173"/>
+      <c r="A28" s="168"/>
       <c r="B28" s="75" t="s">
         <v>51</v>
       </c>
@@ -16641,7 +16900,7 @@
       <c r="AML28" s="81"/>
     </row>
     <row r="29" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="173"/>
+      <c r="A29" s="168"/>
       <c r="B29" s="75" t="s">
         <v>52</v>
       </c>
@@ -17679,7 +17938,7 @@
       <c r="AML29" s="81"/>
     </row>
     <row r="30" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="173"/>
+      <c r="A30" s="168"/>
       <c r="B30" s="75" t="s">
         <v>53</v>
       </c>
@@ -18717,7 +18976,7 @@
       <c r="AML30" s="81"/>
     </row>
     <row r="31" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="172">
+      <c r="A31" s="167">
         <v>6</v>
       </c>
       <c r="B31" s="74" t="s">
@@ -18738,7 +18997,7 @@
       <c r="G31" s="77"/>
     </row>
     <row r="32" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="173"/>
+      <c r="A32" s="168"/>
       <c r="B32" s="75" t="s">
         <v>55</v>
       </c>
@@ -18757,7 +19016,7 @@
       <c r="G32" s="78"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="173"/>
+      <c r="A33" s="168"/>
       <c r="B33" s="75" t="s">
         <v>56</v>
       </c>
@@ -18776,7 +19035,7 @@
       <c r="G33" s="78"/>
     </row>
     <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="172">
+      <c r="A34" s="167">
         <v>7</v>
       </c>
       <c r="B34" s="74" t="s">
@@ -18797,7 +19056,7 @@
       <c r="G34" s="77"/>
     </row>
     <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="173"/>
+      <c r="A35" s="168"/>
       <c r="B35" s="75" t="s">
         <v>57</v>
       </c>
@@ -18816,7 +19075,7 @@
       <c r="G35" s="78"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="173"/>
+      <c r="A36" s="168"/>
       <c r="B36" s="75" t="s">
         <v>58</v>
       </c>
@@ -18835,7 +19094,7 @@
       <c r="G36" s="78"/>
     </row>
     <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="174"/>
+      <c r="A37" s="169"/>
       <c r="B37" s="76"/>
       <c r="C37" s="44"/>
       <c r="D37" s="45"/>
@@ -18844,7 +19103,7 @@
       <c r="G37" s="79"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="172"/>
+      <c r="A38" s="167"/>
       <c r="B38" s="74"/>
       <c r="C38" s="39"/>
       <c r="D38" s="40"/>
@@ -18853,7 +19112,7 @@
       <c r="G38" s="77"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="173"/>
+      <c r="A39" s="168"/>
       <c r="B39" s="75"/>
       <c r="C39" s="42"/>
       <c r="D39" s="28"/>
@@ -18862,7 +19121,7 @@
       <c r="G39" s="78"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="173"/>
+      <c r="A40" s="168"/>
       <c r="B40" s="75"/>
       <c r="C40" s="42"/>
       <c r="D40" s="28"/>
@@ -18871,7 +19130,7 @@
       <c r="G40" s="78"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="173"/>
+      <c r="A41" s="168"/>
       <c r="B41" s="75"/>
       <c r="C41" s="42"/>
       <c r="D41" s="28"/>
@@ -18880,7 +19139,7 @@
       <c r="G41" s="78"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="174"/>
+      <c r="A42" s="169"/>
       <c r="B42" s="76"/>
       <c r="C42" s="44"/>
       <c r="D42" s="45"/>
@@ -18889,7 +19148,7 @@
       <c r="G42" s="79"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="172"/>
+      <c r="A43" s="167"/>
       <c r="B43" s="74"/>
       <c r="C43" s="39"/>
       <c r="D43" s="40"/>
@@ -18898,7 +19157,7 @@
       <c r="G43" s="77"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="173"/>
+      <c r="A44" s="168"/>
       <c r="B44" s="75"/>
       <c r="C44" s="42"/>
       <c r="D44" s="28"/>
@@ -18907,7 +19166,7 @@
       <c r="G44" s="78"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="173"/>
+      <c r="A45" s="168"/>
       <c r="B45" s="75"/>
       <c r="C45" s="42"/>
       <c r="D45" s="28"/>
@@ -18916,7 +19175,7 @@
       <c r="G45" s="78"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="173"/>
+      <c r="A46" s="168"/>
       <c r="B46" s="75"/>
       <c r="C46" s="42"/>
       <c r="D46" s="28"/>
@@ -18925,7 +19184,7 @@
       <c r="G46" s="78"/>
     </row>
     <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="174"/>
+      <c r="A47" s="169"/>
       <c r="B47" s="76"/>
       <c r="C47" s="44"/>
       <c r="D47" s="45"/>
@@ -18956,7 +19215,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18969,16 +19228,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="166" t="s">
+      <c r="A1" s="161" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
+      <c r="B1" s="161"/>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="161"/>
+      <c r="G1" s="161"/>
+      <c r="H1" s="161"/>
     </row>
     <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="48" t="s">
@@ -19004,25 +19263,25 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="176" t="s">
+      <c r="A3" s="171" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="179" t="s">
+      <c r="B3" s="174" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="148">
+      <c r="C3" s="143">
         <v>1</v>
       </c>
-      <c r="D3" s="147" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" s="138"/>
-      <c r="F3" s="137"/>
-      <c r="G3" s="137"/>
+      <c r="D3" s="142" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="137"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="136"/>
     </row>
     <row r="4" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="177"/>
-      <c r="B4" s="156"/>
+      <c r="A4" s="172"/>
+      <c r="B4" s="151"/>
       <c r="C4" s="129">
         <v>2</v>
       </c>
@@ -19034,12 +19293,12 @@
       <c r="G4" s="131"/>
     </row>
     <row r="5" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="177"/>
-      <c r="B5" s="156"/>
+      <c r="A5" s="172"/>
+      <c r="B5" s="151"/>
       <c r="C5" s="129">
         <v>3</v>
       </c>
-      <c r="D5" s="135" t="s">
+      <c r="D5" s="197" t="s">
         <v>41</v>
       </c>
       <c r="E5" s="130"/>
@@ -19047,12 +19306,12 @@
       <c r="G5" s="131"/>
     </row>
     <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="178"/>
-      <c r="B6" s="180"/>
+      <c r="A6" s="173"/>
+      <c r="B6" s="175"/>
       <c r="C6" s="129">
         <v>4</v>
       </c>
-      <c r="D6" s="135" t="s">
+      <c r="D6" s="197" t="s">
         <v>40</v>
       </c>
       <c r="E6" s="130"/>
@@ -19087,10 +19346,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19123,344 +19382,381 @@
       <c r="F2" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="140" t="s">
+      <c r="G2" s="138" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="181">
+    <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="177">
         <v>1</v>
       </c>
-      <c r="B3" s="139" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="141" t="s">
+      <c r="B3" s="194" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="195" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="141" t="s">
+      <c r="D3" s="195" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="141" t="s">
+      <c r="E3" s="195" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="142" t="s">
+      <c r="F3" s="196" t="s">
         <v>76</v>
       </c>
-      <c r="G3" s="143"/>
+      <c r="G3" s="181"/>
     </row>
     <row r="4" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="182"/>
-      <c r="B4" s="144" t="s">
-        <v>95</v>
-      </c>
-      <c r="C4" s="141" t="s">
+      <c r="A4" s="177"/>
+      <c r="B4" s="185" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="179" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="141" t="s">
+      <c r="D4" s="179" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="141" t="s">
+      <c r="E4" s="179" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="145" t="s">
+      <c r="F4" s="186" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="146"/>
+      <c r="G4" s="180"/>
     </row>
     <row r="5" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="182"/>
-      <c r="B5" s="144" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" s="141" t="s">
+      <c r="A5" s="177"/>
+      <c r="B5" s="187" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="141" t="s">
+      <c r="D5" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="141" t="s">
+      <c r="E5" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="145" t="s">
+      <c r="F5" s="188" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="146"/>
+      <c r="G5" s="141"/>
     </row>
     <row r="6" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="181">
-        <v>2</v>
-      </c>
-      <c r="B6" s="139" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="141" t="s">
+      <c r="A6" s="178"/>
+      <c r="B6" s="187" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="141" t="s">
+      <c r="D6" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="141" t="s">
+      <c r="E6" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="142" t="s">
+      <c r="F6" s="188" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="143"/>
+      <c r="G6" s="141"/>
     </row>
     <row r="7" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="182"/>
-      <c r="B7" s="144" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="141" t="s">
+      <c r="A7" s="182">
+        <v>2</v>
+      </c>
+      <c r="B7" s="189" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="141" t="s">
+      <c r="D7" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="141" t="s">
+      <c r="E7" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="145" t="s">
+      <c r="F7" s="190" t="s">
         <v>76</v>
       </c>
-      <c r="G7" s="146"/>
+      <c r="G7" s="140"/>
     </row>
     <row r="8" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="182"/>
-      <c r="B8" s="144" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="141" t="s">
+      <c r="A8" s="183"/>
+      <c r="B8" s="187" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="141" t="s">
+      <c r="D8" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="141" t="s">
+      <c r="E8" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="145" t="s">
+      <c r="F8" s="188" t="s">
         <v>76</v>
       </c>
-      <c r="G8" s="146"/>
+      <c r="G8" s="141"/>
     </row>
     <row r="9" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="181">
-        <v>3</v>
-      </c>
-      <c r="B9" s="139" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="141" t="s">
+      <c r="A9" s="183"/>
+      <c r="B9" s="187" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="141" t="s">
+      <c r="D9" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="141" t="s">
+      <c r="E9" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="142" t="s">
+      <c r="F9" s="188" t="s">
         <v>76</v>
       </c>
-      <c r="G9" s="143"/>
+      <c r="G9" s="141"/>
     </row>
     <row r="10" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="182"/>
-      <c r="B10" s="144" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" s="141" t="s">
+      <c r="A10" s="182">
+        <v>3</v>
+      </c>
+      <c r="B10" s="189" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="141" t="s">
+      <c r="D10" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="141" t="s">
+      <c r="E10" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="145"/>
-      <c r="G10" s="146"/>
+      <c r="F10" s="190" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" s="140"/>
     </row>
     <row r="11" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="182"/>
-      <c r="B11" s="144" t="s">
+      <c r="A11" s="183"/>
+      <c r="B11" s="187" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="139" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="139" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="139" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="188" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="141"/>
+    </row>
+    <row r="12" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="183"/>
+      <c r="B12" s="187" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="139" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="139" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="139" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="188" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="141"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="183"/>
+      <c r="B13" s="187" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="141" t="s">
+      <c r="C13" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="141" t="s">
+      <c r="D13" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="141" t="s">
+      <c r="E13" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="145"/>
-      <c r="G11" s="146"/>
+      <c r="F13" s="188" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="141"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="182"/>
-      <c r="B12" s="144" t="s">
+    <row r="14" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="182">
+        <v>4</v>
+      </c>
+      <c r="B14" s="189" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="141" t="s">
+      <c r="C14" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="141" t="s">
+      <c r="D14" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="141" t="s">
+      <c r="E14" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="145"/>
-      <c r="G12" s="146"/>
+      <c r="F14" s="190" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" s="140"/>
     </row>
-    <row r="13" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="181">
-        <v>4</v>
-      </c>
-      <c r="B13" s="139" t="s">
+    <row r="15" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="183"/>
+      <c r="B15" s="187" t="s">
         <v>88</v>
       </c>
-      <c r="C13" s="141" t="s">
+      <c r="C15" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="141" t="s">
+      <c r="D15" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="141" t="s">
+      <c r="E15" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="142" t="s">
+      <c r="F15" s="188" t="s">
         <v>76</v>
       </c>
-      <c r="G13" s="143"/>
-    </row>
-    <row r="14" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="182"/>
-      <c r="B14" s="144" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" s="141" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="141" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="141" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="145"/>
-      <c r="G14" s="146"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="182"/>
-      <c r="B15" s="144" t="s">
-        <v>90</v>
-      </c>
-      <c r="C15" s="141" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="141" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="141" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="145"/>
-      <c r="G15" s="146"/>
+      <c r="G15" s="141"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="182"/>
-      <c r="B16" s="144" t="s">
-        <v>91</v>
-      </c>
-      <c r="C16" s="141" t="s">
+      <c r="A16" s="183"/>
+      <c r="B16" s="187" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="141" t="s">
+      <c r="D16" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="141" t="s">
+      <c r="E16" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="145"/>
-      <c r="G16" s="146"/>
+      <c r="F16" s="188" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="141"/>
     </row>
-    <row r="17" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="181">
-        <v>5</v>
-      </c>
-      <c r="B17" s="139" t="s">
-        <v>92</v>
-      </c>
-      <c r="C17" s="141" t="s">
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="183"/>
+      <c r="B17" s="187" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="141" t="s">
+      <c r="D17" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="141" t="s">
+      <c r="E17" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="142"/>
-      <c r="G17" s="143"/>
+      <c r="F17" s="188" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="141"/>
     </row>
     <row r="18" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="182"/>
-      <c r="B18" s="144" t="s">
+      <c r="A18" s="182">
+        <v>5</v>
+      </c>
+      <c r="B18" s="189" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="139" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="139" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="139" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="190" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18" s="140"/>
+    </row>
+    <row r="19" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="183"/>
+      <c r="B19" s="187" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="139" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="139" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="139" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="188" t="s">
+        <v>76</v>
+      </c>
+      <c r="G19" s="141"/>
+    </row>
+    <row r="20" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="183"/>
+      <c r="B20" s="191" t="s">
         <v>93</v>
       </c>
-      <c r="C18" s="141" t="s">
+      <c r="C20" s="192" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="141" t="s">
+      <c r="D20" s="192" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="141" t="s">
+      <c r="E20" s="192" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="145"/>
-      <c r="G18" s="146"/>
+      <c r="F20" s="193" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20" s="141"/>
     </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A19" s="182"/>
-      <c r="B19" s="144" t="s">
-        <v>94</v>
-      </c>
-      <c r="C19" s="141" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="141" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="141" t="s">
-        <v>49</v>
-      </c>
-      <c r="F19" s="145"/>
-      <c r="G19" s="146"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="136"/>
-      <c r="B20" s="136"/>
-      <c r="C20" s="136"/>
-      <c r="D20" s="136"/>
-      <c r="E20" s="136"/>
-      <c r="F20" s="136"/>
-      <c r="G20" s="136"/>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="135"/>
+      <c r="B21" s="184"/>
+      <c r="C21" s="184"/>
+      <c r="D21" s="184"/>
+      <c r="E21" s="184"/>
+      <c r="F21" s="184"/>
+      <c r="G21" s="135"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A3:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Finished admin vip removal Finished VIP flat rate discount
</commit_message>
<xml_diff>
--- a/jasonH-wsp21-ProductSprintBackLog.xlsx
+++ b/jasonH-wsp21-ProductSprintBackLog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="1035" windowWidth="21600" windowHeight="11265" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="7200" yWindow="1035" windowWidth="21600" windowHeight="11265" tabRatio="500" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Proposed Product Backlog" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="115">
   <si>
     <t>Category</t>
   </si>
@@ -353,6 +353,57 @@
   <si>
     <t>Guest can view comments before signing in</t>
   </si>
+  <si>
+    <t>There is a button on the product cards to add to wishlist</t>
+  </si>
+  <si>
+    <t>When clicking the button the product is added to the user's wishlist</t>
+  </si>
+  <si>
+    <t>When not signed there is no button for wishlisting</t>
+  </si>
+  <si>
+    <t>&lt;As a&gt; user &lt; I want&gt; a wishlist button &lt;so that&gt; I can view my wishlist</t>
+  </si>
+  <si>
+    <t>When viewing the product page as a guest the wishlist button does not display</t>
+  </si>
+  <si>
+    <t>When signing in the wishlist button is visible</t>
+  </si>
+  <si>
+    <t>The user is directed to their wishlist when clicking the wishlist button</t>
+  </si>
+  <si>
+    <t>On the wishlist page there is a remove item button</t>
+  </si>
+  <si>
+    <t>The user can click the remove item button to remove the item</t>
+  </si>
+  <si>
+    <t>Once the user removes the item it is removed from the page and firebase</t>
+  </si>
+  <si>
+    <t>On the wishlist page there is an add to cart button</t>
+  </si>
+  <si>
+    <t>When the user clicks the add to cart button it is removed from the wishlist</t>
+  </si>
+  <si>
+    <t>When the user clicks the add to cart button it is added to the user's shopping cart</t>
+  </si>
+  <si>
+    <t>When the user views the home page the products are displayed through pages of products</t>
+  </si>
+  <si>
+    <t>On the home page there is a next page button</t>
+  </si>
+  <si>
+    <t>On the home page there is a previous page button</t>
+  </si>
+  <si>
+    <t>A page holds 8 products</t>
+  </si>
 </sst>
 </file>
 
@@ -474,7 +525,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -499,8 +550,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="78">
+  <borders count="89">
     <border>
       <left/>
       <right/>
@@ -1503,11 +1560,120 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="198">
+  <cellXfs count="223">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1842,6 +2008,55 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1911,6 +2126,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1918,9 +2136,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1938,8 +2153,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1947,61 +2165,82 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2320,7 +2559,7 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8:B10"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2357,10 +2596,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="148" t="s">
+      <c r="A2" s="165" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="150" t="s">
+      <c r="B2" s="167" t="s">
         <v>47</v>
       </c>
       <c r="C2" s="56">
@@ -2374,8 +2613,8 @@
       <c r="G2" s="58"/>
     </row>
     <row r="3" spans="1:7" s="89" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="149"/>
-      <c r="B3" s="151"/>
+      <c r="A3" s="166"/>
+      <c r="B3" s="168"/>
       <c r="C3" s="84">
         <v>2</v>
       </c>
@@ -2387,8 +2626,8 @@
       <c r="G3" s="86"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="149"/>
-      <c r="B4" s="151"/>
+      <c r="A4" s="166"/>
+      <c r="B4" s="168"/>
       <c r="C4" s="84">
         <v>3</v>
       </c>
@@ -2400,14 +2639,14 @@
       <c r="G4" s="86"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="149"/>
-      <c r="B5" s="151" t="s">
+      <c r="A5" s="166"/>
+      <c r="B5" s="199" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="84">
         <v>4</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="200" t="s">
         <v>32</v>
       </c>
       <c r="E5" s="83"/>
@@ -2415,12 +2654,12 @@
       <c r="G5" s="86"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="149"/>
-      <c r="B6" s="151"/>
+      <c r="A6" s="166"/>
+      <c r="B6" s="199"/>
       <c r="C6" s="84">
         <v>5</v>
       </c>
-      <c r="D6" s="104" t="s">
+      <c r="D6" s="201" t="s">
         <v>33</v>
       </c>
       <c r="E6" s="83"/>
@@ -2428,12 +2667,12 @@
       <c r="G6" s="86"/>
     </row>
     <row r="7" spans="1:7" s="90" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="149"/>
-      <c r="B7" s="151"/>
+      <c r="A7" s="166"/>
+      <c r="B7" s="199"/>
       <c r="C7" s="84">
         <v>6</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="200" t="s">
         <v>34</v>
       </c>
       <c r="E7" s="83"/>
@@ -2441,8 +2680,8 @@
       <c r="G7" s="86"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="149"/>
-      <c r="B8" s="152" t="s">
+      <c r="A8" s="166"/>
+      <c r="B8" s="169" t="s">
         <v>38</v>
       </c>
       <c r="C8" s="84">
@@ -2456,8 +2695,8 @@
       <c r="G8" s="86"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="149"/>
-      <c r="B9" s="152"/>
+      <c r="A9" s="166"/>
+      <c r="B9" s="169"/>
       <c r="C9" s="84">
         <v>8</v>
       </c>
@@ -2469,8 +2708,8 @@
       <c r="G9" s="86"/>
     </row>
     <row r="10" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="149"/>
-      <c r="B10" s="152"/>
+      <c r="A10" s="166"/>
+      <c r="B10" s="169"/>
       <c r="C10" s="84">
         <v>9</v>
       </c>
@@ -2482,7 +2721,7 @@
       <c r="G10" s="86"/>
     </row>
     <row r="11" spans="1:7" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="149"/>
+      <c r="A11" s="166"/>
       <c r="B11" s="114"/>
       <c r="C11" s="84">
         <v>10</v>
@@ -2495,7 +2734,7 @@
       <c r="G11" s="86"/>
     </row>
     <row r="12" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="149"/>
+      <c r="A12" s="166"/>
       <c r="B12" s="114"/>
       <c r="C12" s="84">
         <v>11</v>
@@ -2508,12 +2747,12 @@
       <c r="G12" s="86"/>
     </row>
     <row r="13" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="149"/>
+      <c r="A13" s="166"/>
       <c r="B13" s="102"/>
       <c r="C13" s="53">
         <v>12</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="200" t="s">
         <v>42</v>
       </c>
       <c r="E13" s="54"/>
@@ -2522,7 +2761,7 @@
     </row>
     <row r="14" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="110"/>
-      <c r="B14" s="153" t="s">
+      <c r="B14" s="170" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="111">
@@ -2536,10 +2775,10 @@
       <c r="G14" s="62"/>
     </row>
     <row r="15" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="156" t="s">
+      <c r="A15" s="173" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="154"/>
+      <c r="B15" s="171"/>
       <c r="C15" s="59">
         <v>14</v>
       </c>
@@ -2551,8 +2790,8 @@
       <c r="G15" s="61"/>
     </row>
     <row r="16" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="157"/>
-      <c r="B16" s="154"/>
+      <c r="A16" s="174"/>
+      <c r="B16" s="171"/>
       <c r="C16" s="91">
         <v>15</v>
       </c>
@@ -2564,8 +2803,8 @@
       <c r="G16" s="93"/>
     </row>
     <row r="17" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="157"/>
-      <c r="B17" s="154"/>
+      <c r="A17" s="174"/>
+      <c r="B17" s="171"/>
       <c r="C17" s="91">
         <v>16</v>
       </c>
@@ -2577,8 +2816,8 @@
       <c r="G17" s="93"/>
     </row>
     <row r="18" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="157"/>
-      <c r="B18" s="155"/>
+      <c r="A18" s="174"/>
+      <c r="B18" s="172"/>
       <c r="C18" s="63">
         <v>17</v>
       </c>
@@ -2590,8 +2829,8 @@
       <c r="G18" s="65"/>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="157"/>
-      <c r="B19" s="159" t="s">
+      <c r="A19" s="174"/>
+      <c r="B19" s="176" t="s">
         <v>35</v>
       </c>
       <c r="C19" s="98">
@@ -2605,8 +2844,8 @@
       <c r="G19" s="101"/>
     </row>
     <row r="20" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="157"/>
-      <c r="B20" s="159"/>
+      <c r="A20" s="174"/>
+      <c r="B20" s="176"/>
       <c r="C20" s="98">
         <v>19</v>
       </c>
@@ -2618,8 +2857,8 @@
       <c r="G20" s="101"/>
     </row>
     <row r="21" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="158"/>
-      <c r="B21" s="160"/>
+      <c r="A21" s="175"/>
+      <c r="B21" s="177"/>
       <c r="C21" s="106">
         <v>20</v>
       </c>
@@ -2631,8 +2870,8 @@
       <c r="G21" s="109"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="144"/>
-      <c r="B22" s="146"/>
+      <c r="A22" s="161"/>
+      <c r="B22" s="163"/>
       <c r="C22" s="66"/>
       <c r="D22" s="67"/>
       <c r="E22" s="67"/>
@@ -2640,8 +2879,8 @@
       <c r="G22" s="69"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="145"/>
-      <c r="B23" s="147"/>
+      <c r="A23" s="162"/>
+      <c r="B23" s="164"/>
       <c r="C23" s="70"/>
       <c r="D23" s="71"/>
       <c r="E23" s="72"/>
@@ -2683,12 +2922,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" s="24" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="176" t="s">
+      <c r="A3" s="197" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="176"/>
-      <c r="C3" s="176"/>
-      <c r="D3" s="176"/>
+      <c r="B3" s="197"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="197"/>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:4" s="27" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2785,7 +3024,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -2802,16 +3041,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="178" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="161"/>
-      <c r="G1" s="161"/>
-      <c r="H1" s="161"/>
+      <c r="B1" s="178"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
+      <c r="H1" s="178"/>
       <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -2851,7 +3090,7 @@
       <c r="I3" s="10"/>
     </row>
     <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="148" t="s">
+      <c r="A4" s="165" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="116"/>
@@ -2864,7 +3103,7 @@
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="149"/>
+      <c r="A5" s="166"/>
       <c r="B5" s="102"/>
       <c r="C5" s="84">
         <v>1</v>
@@ -2879,7 +3118,7 @@
       <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="149"/>
+      <c r="A6" s="166"/>
       <c r="B6" s="102"/>
       <c r="C6" s="84"/>
       <c r="D6" s="54"/>
@@ -2890,7 +3129,7 @@
       <c r="I6" s="9"/>
     </row>
     <row r="7" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="149"/>
+      <c r="A7" s="166"/>
       <c r="B7" s="102"/>
       <c r="C7" s="84"/>
       <c r="D7" s="16"/>
@@ -2901,7 +3140,7 @@
       <c r="I7" s="9"/>
     </row>
     <row r="8" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="149"/>
+      <c r="A8" s="166"/>
       <c r="B8" s="102"/>
       <c r="C8" s="84"/>
       <c r="D8" s="104"/>
@@ -2912,7 +3151,7 @@
       <c r="I8" s="9"/>
     </row>
     <row r="9" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="149"/>
+      <c r="A9" s="166"/>
       <c r="B9" s="102"/>
       <c r="C9" s="84"/>
       <c r="D9" s="16"/>
@@ -2923,7 +3162,7 @@
       <c r="I9" s="9"/>
     </row>
     <row r="10" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="149"/>
+      <c r="A10" s="166"/>
       <c r="B10" s="102"/>
       <c r="C10" s="84"/>
       <c r="D10" s="16"/>
@@ -2934,7 +3173,7 @@
       <c r="I10" s="9"/>
     </row>
     <row r="11" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="149"/>
+      <c r="A11" s="166"/>
       <c r="B11" s="102"/>
       <c r="C11" s="84"/>
       <c r="D11" s="16"/>
@@ -2945,7 +3184,7 @@
       <c r="I11" s="9"/>
     </row>
     <row r="12" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="149"/>
+      <c r="A12" s="166"/>
       <c r="B12" s="102"/>
       <c r="C12" s="84"/>
       <c r="D12" s="16"/>
@@ -2956,7 +3195,7 @@
       <c r="I12" s="9"/>
     </row>
     <row r="13" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="149"/>
+      <c r="A13" s="166"/>
       <c r="B13" s="103"/>
       <c r="C13" s="84"/>
       <c r="D13" s="16"/>
@@ -2967,7 +3206,7 @@
       <c r="I13" s="9"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="149"/>
+      <c r="A14" s="166"/>
       <c r="B14" s="103"/>
       <c r="C14" s="84"/>
       <c r="D14" s="16"/>
@@ -2978,7 +3217,7 @@
       <c r="I14" s="9"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="149"/>
+      <c r="A15" s="166"/>
       <c r="B15" s="102"/>
       <c r="C15" s="53"/>
       <c r="D15" s="16"/>
@@ -2988,10 +3227,10 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="165" t="s">
+      <c r="A16" s="182" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="159" t="s">
+      <c r="B16" s="176" t="s">
         <v>35</v>
       </c>
       <c r="C16" s="111">
@@ -3006,8 +3245,8 @@
       <c r="H16" s="16"/>
     </row>
     <row r="17" spans="1:9" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="149"/>
-      <c r="B17" s="159"/>
+      <c r="A17" s="166"/>
+      <c r="B17" s="176"/>
       <c r="C17" s="59">
         <v>3</v>
       </c>
@@ -3021,8 +3260,8 @@
       <c r="I17" s="9"/>
     </row>
     <row r="18" spans="1:9" ht="26.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="149"/>
-      <c r="B18" s="160"/>
+      <c r="A18" s="166"/>
+      <c r="B18" s="177"/>
       <c r="C18" s="91">
         <v>4</v>
       </c>
@@ -3036,8 +3275,8 @@
       <c r="I18" s="9"/>
     </row>
     <row r="19" spans="1:9" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="149"/>
-      <c r="B19" s="153" t="s">
+      <c r="A19" s="166"/>
+      <c r="B19" s="170" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="91">
@@ -3053,8 +3292,8 @@
       <c r="I19" s="9"/>
     </row>
     <row r="20" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="149"/>
-      <c r="B20" s="154"/>
+      <c r="A20" s="166"/>
+      <c r="B20" s="171"/>
       <c r="C20" s="63">
         <v>6</v>
       </c>
@@ -3066,8 +3305,8 @@
       <c r="G20" s="65"/>
     </row>
     <row r="21" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="149"/>
-      <c r="B21" s="154"/>
+      <c r="A21" s="166"/>
+      <c r="B21" s="171"/>
       <c r="C21" s="98">
         <v>7</v>
       </c>
@@ -3079,8 +3318,8 @@
       <c r="G21" s="101"/>
     </row>
     <row r="22" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="149"/>
-      <c r="B22" s="154"/>
+      <c r="A22" s="166"/>
+      <c r="B22" s="171"/>
       <c r="C22" s="98"/>
       <c r="D22" s="64"/>
       <c r="E22" s="99"/>
@@ -3088,8 +3327,8 @@
       <c r="G22" s="101"/>
     </row>
     <row r="23" spans="1:9" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="166"/>
-      <c r="B23" s="155"/>
+      <c r="A23" s="183"/>
+      <c r="B23" s="172"/>
       <c r="C23" s="106"/>
       <c r="D23" s="105"/>
       <c r="E23" s="107"/>
@@ -3097,8 +3336,8 @@
       <c r="G23" s="109"/>
     </row>
     <row r="24" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="144"/>
-      <c r="B24" s="146"/>
+      <c r="A24" s="161"/>
+      <c r="B24" s="163"/>
       <c r="C24" s="66"/>
       <c r="D24" s="67"/>
       <c r="E24" s="67"/>
@@ -3106,8 +3345,8 @@
       <c r="G24" s="69"/>
     </row>
     <row r="25" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="145"/>
-      <c r="B25" s="147"/>
+      <c r="A25" s="162"/>
+      <c r="B25" s="164"/>
       <c r="C25" s="70"/>
       <c r="D25" s="71"/>
       <c r="E25" s="72"/>
@@ -3115,38 +3354,38 @@
       <c r="G25" s="73"/>
     </row>
     <row r="26" spans="1:9" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="163" t="s">
+      <c r="A26" s="180" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="163"/>
-      <c r="C26" s="163"/>
-      <c r="D26" s="163"/>
+      <c r="B26" s="180"/>
+      <c r="C26" s="180"/>
+      <c r="D26" s="180"/>
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
       <c r="G26" s="18"/>
       <c r="H26" s="17"/>
     </row>
     <row r="27" spans="1:9" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="164" t="s">
+      <c r="A27" s="181" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="164"/>
-      <c r="C27" s="164"/>
-      <c r="D27" s="164"/>
-      <c r="E27" s="164"/>
-      <c r="F27" s="164"/>
-      <c r="G27" s="164"/>
+      <c r="B27" s="181"/>
+      <c r="C27" s="181"/>
+      <c r="D27" s="181"/>
+      <c r="E27" s="181"/>
+      <c r="F27" s="181"/>
+      <c r="G27" s="181"/>
       <c r="H27" s="20"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="162" t="s">
+      <c r="A28" s="179" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="162"/>
-      <c r="C28" s="162"/>
-      <c r="D28" s="162"/>
-      <c r="E28" s="162"/>
-      <c r="F28" s="162"/>
+      <c r="B28" s="179"/>
+      <c r="C28" s="179"/>
+      <c r="D28" s="179"/>
+      <c r="E28" s="179"/>
+      <c r="F28" s="179"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3170,7 +3409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AML47"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A38" sqref="A38:G42"/>
     </sheetView>
   </sheetViews>
@@ -3209,7 +3448,7 @@
       </c>
     </row>
     <row r="3" spans="1:1026" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="170"/>
+      <c r="A3" s="184"/>
       <c r="B3" s="29"/>
       <c r="C3" s="39"/>
       <c r="D3" s="39"/>
@@ -3218,7 +3457,7 @@
       <c r="G3" s="32"/>
     </row>
     <row r="4" spans="1:1026" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="170"/>
+      <c r="A4" s="184"/>
       <c r="B4" s="30"/>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
@@ -3227,7 +3466,7 @@
       <c r="G4" s="33"/>
     </row>
     <row r="5" spans="1:1026" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="170"/>
+      <c r="A5" s="184"/>
       <c r="B5" s="96"/>
       <c r="C5" s="39"/>
       <c r="D5" s="39"/>
@@ -3236,7 +3475,7 @@
       <c r="G5" s="33"/>
     </row>
     <row r="6" spans="1:1026" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="170"/>
+      <c r="A6" s="184"/>
       <c r="B6" s="96"/>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
@@ -3245,7 +3484,7 @@
       <c r="G6" s="33"/>
     </row>
     <row r="7" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="170"/>
+      <c r="A7" s="184"/>
       <c r="B7" s="31"/>
       <c r="C7" s="39"/>
       <c r="D7" s="39"/>
@@ -3254,7 +3493,7 @@
       <c r="G7" s="34"/>
     </row>
     <row r="8" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="170"/>
+      <c r="A8" s="184"/>
       <c r="B8" s="97"/>
       <c r="C8" s="39"/>
       <c r="D8" s="39"/>
@@ -3263,7 +3502,7 @@
       <c r="G8" s="35"/>
     </row>
     <row r="9" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="170">
+      <c r="A9" s="184">
         <v>1</v>
       </c>
       <c r="B9" s="120" t="s">
@@ -3284,7 +3523,7 @@
       <c r="G9" s="36"/>
     </row>
     <row r="10" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="170"/>
+      <c r="A10" s="184"/>
       <c r="B10" s="30" t="s">
         <v>65</v>
       </c>
@@ -3303,7 +3542,7 @@
       <c r="G10" s="37"/>
     </row>
     <row r="11" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="170"/>
+      <c r="A11" s="184"/>
       <c r="B11" s="30" t="s">
         <v>67</v>
       </c>
@@ -3322,7 +3561,7 @@
       <c r="G11" s="37"/>
     </row>
     <row r="12" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="170"/>
+      <c r="A12" s="184"/>
       <c r="B12" s="21" t="s">
         <v>77</v>
       </c>
@@ -3341,7 +3580,7 @@
       <c r="G12" s="37"/>
     </row>
     <row r="13" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="170"/>
+      <c r="A13" s="184"/>
       <c r="B13" s="30" t="s">
         <v>66</v>
       </c>
@@ -3360,7 +3599,7 @@
       <c r="G13" s="35"/>
     </row>
     <row r="14" spans="1:1026" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="170">
+      <c r="A14" s="184">
         <v>2</v>
       </c>
       <c r="B14" s="29" t="s">
@@ -3381,7 +3620,7 @@
       <c r="G14" s="32"/>
     </row>
     <row r="15" spans="1:1026" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="170"/>
+      <c r="A15" s="184"/>
       <c r="B15" s="117" t="s">
         <v>60</v>
       </c>
@@ -4419,7 +4658,7 @@
       <c r="AML15" s="115"/>
     </row>
     <row r="16" spans="1:1026" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="170"/>
+      <c r="A16" s="184"/>
       <c r="B16" s="117" t="s">
         <v>61</v>
       </c>
@@ -5457,7 +5696,7 @@
       <c r="AML16" s="115"/>
     </row>
     <row r="17" spans="1:1026" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="170"/>
+      <c r="A17" s="184"/>
       <c r="B17" s="117" t="s">
         <v>63</v>
       </c>
@@ -6495,7 +6734,7 @@
       <c r="AML17" s="115"/>
     </row>
     <row r="18" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="170"/>
+      <c r="A18" s="184"/>
       <c r="B18" s="96" t="s">
         <v>64</v>
       </c>
@@ -6514,7 +6753,7 @@
       <c r="G18" s="37"/>
     </row>
     <row r="19" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="167">
+      <c r="A19" s="185">
         <v>3</v>
       </c>
       <c r="B19" s="74" t="s">
@@ -7554,7 +7793,7 @@
       <c r="AML19" s="81"/>
     </row>
     <row r="20" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="168"/>
+      <c r="A20" s="186"/>
       <c r="B20" s="75" t="s">
         <v>69</v>
       </c>
@@ -8592,7 +8831,7 @@
       <c r="AML20" s="81"/>
     </row>
     <row r="21" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="168"/>
+      <c r="A21" s="186"/>
       <c r="B21" s="75" t="s">
         <v>70</v>
       </c>
@@ -9630,7 +9869,7 @@
       <c r="AML21" s="81"/>
     </row>
     <row r="22" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="167">
+      <c r="A22" s="185">
         <v>4</v>
       </c>
       <c r="B22" s="74" t="s">
@@ -10670,7 +10909,7 @@
       <c r="AML22" s="81"/>
     </row>
     <row r="23" spans="1:1026" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="168"/>
+      <c r="A23" s="186"/>
       <c r="B23" s="75" t="s">
         <v>72</v>
       </c>
@@ -11708,7 +11947,7 @@
       <c r="AML23" s="81"/>
     </row>
     <row r="24" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="168"/>
+      <c r="A24" s="186"/>
       <c r="B24" s="75" t="s">
         <v>73</v>
       </c>
@@ -12746,7 +12985,7 @@
       <c r="AML24" s="81"/>
     </row>
     <row r="25" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="168"/>
+      <c r="A25" s="186"/>
       <c r="B25" s="75" t="s">
         <v>74</v>
       </c>
@@ -13784,7 +14023,7 @@
       <c r="AML25" s="81"/>
     </row>
     <row r="26" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="169"/>
+      <c r="A26" s="187"/>
       <c r="B26" s="76" t="s">
         <v>75</v>
       </c>
@@ -14822,7 +15061,7 @@
       <c r="AML26" s="81"/>
     </row>
     <row r="27" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="167">
+      <c r="A27" s="185">
         <v>5</v>
       </c>
       <c r="B27" s="74" t="s">
@@ -15862,7 +16101,7 @@
       <c r="AML27" s="81"/>
     </row>
     <row r="28" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="168"/>
+      <c r="A28" s="186"/>
       <c r="B28" s="75" t="s">
         <v>51</v>
       </c>
@@ -16900,7 +17139,7 @@
       <c r="AML28" s="81"/>
     </row>
     <row r="29" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="168"/>
+      <c r="A29" s="186"/>
       <c r="B29" s="75" t="s">
         <v>52</v>
       </c>
@@ -17938,7 +18177,7 @@
       <c r="AML29" s="81"/>
     </row>
     <row r="30" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="168"/>
+      <c r="A30" s="186"/>
       <c r="B30" s="75" t="s">
         <v>53</v>
       </c>
@@ -18976,7 +19215,7 @@
       <c r="AML30" s="81"/>
     </row>
     <row r="31" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="167">
+      <c r="A31" s="185">
         <v>6</v>
       </c>
       <c r="B31" s="74" t="s">
@@ -18997,7 +19236,7 @@
       <c r="G31" s="77"/>
     </row>
     <row r="32" spans="1:1026" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="168"/>
+      <c r="A32" s="186"/>
       <c r="B32" s="75" t="s">
         <v>55</v>
       </c>
@@ -19016,7 +19255,7 @@
       <c r="G32" s="78"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="168"/>
+      <c r="A33" s="186"/>
       <c r="B33" s="75" t="s">
         <v>56</v>
       </c>
@@ -19035,7 +19274,7 @@
       <c r="G33" s="78"/>
     </row>
     <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="167">
+      <c r="A34" s="185">
         <v>7</v>
       </c>
       <c r="B34" s="74" t="s">
@@ -19056,7 +19295,7 @@
       <c r="G34" s="77"/>
     </row>
     <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="168"/>
+      <c r="A35" s="186"/>
       <c r="B35" s="75" t="s">
         <v>57</v>
       </c>
@@ -19075,7 +19314,7 @@
       <c r="G35" s="78"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="168"/>
+      <c r="A36" s="186"/>
       <c r="B36" s="75" t="s">
         <v>58</v>
       </c>
@@ -19094,7 +19333,7 @@
       <c r="G36" s="78"/>
     </row>
     <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="169"/>
+      <c r="A37" s="187"/>
       <c r="B37" s="76"/>
       <c r="C37" s="44"/>
       <c r="D37" s="45"/>
@@ -19103,7 +19342,7 @@
       <c r="G37" s="79"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="167"/>
+      <c r="A38" s="185"/>
       <c r="B38" s="74"/>
       <c r="C38" s="39"/>
       <c r="D38" s="40"/>
@@ -19112,7 +19351,7 @@
       <c r="G38" s="77"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="168"/>
+      <c r="A39" s="186"/>
       <c r="B39" s="75"/>
       <c r="C39" s="42"/>
       <c r="D39" s="28"/>
@@ -19121,7 +19360,7 @@
       <c r="G39" s="78"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="168"/>
+      <c r="A40" s="186"/>
       <c r="B40" s="75"/>
       <c r="C40" s="42"/>
       <c r="D40" s="28"/>
@@ -19130,7 +19369,7 @@
       <c r="G40" s="78"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="168"/>
+      <c r="A41" s="186"/>
       <c r="B41" s="75"/>
       <c r="C41" s="42"/>
       <c r="D41" s="28"/>
@@ -19139,7 +19378,7 @@
       <c r="G41" s="78"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="169"/>
+      <c r="A42" s="187"/>
       <c r="B42" s="76"/>
       <c r="C42" s="44"/>
       <c r="D42" s="45"/>
@@ -19148,7 +19387,7 @@
       <c r="G42" s="79"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="167"/>
+      <c r="A43" s="185"/>
       <c r="B43" s="74"/>
       <c r="C43" s="39"/>
       <c r="D43" s="40"/>
@@ -19157,7 +19396,7 @@
       <c r="G43" s="77"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="168"/>
+      <c r="A44" s="186"/>
       <c r="B44" s="75"/>
       <c r="C44" s="42"/>
       <c r="D44" s="28"/>
@@ -19166,7 +19405,7 @@
       <c r="G44" s="78"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="168"/>
+      <c r="A45" s="186"/>
       <c r="B45" s="75"/>
       <c r="C45" s="42"/>
       <c r="D45" s="28"/>
@@ -19175,7 +19414,7 @@
       <c r="G45" s="78"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="168"/>
+      <c r="A46" s="186"/>
       <c r="B46" s="75"/>
       <c r="C46" s="42"/>
       <c r="D46" s="28"/>
@@ -19184,7 +19423,7 @@
       <c r="G46" s="78"/>
     </row>
     <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="169"/>
+      <c r="A47" s="187"/>
       <c r="B47" s="76"/>
       <c r="C47" s="44"/>
       <c r="D47" s="45"/>
@@ -19194,16 +19433,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A43:A47"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A38:A42"/>
     <mergeCell ref="A3:A8"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="A14:A18"/>
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A43:A47"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A38:A42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -19215,7 +19454,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection sqref="A1:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19228,16 +19467,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="178" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="161"/>
-      <c r="G1" s="161"/>
-      <c r="H1" s="161"/>
+      <c r="B1" s="178"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
+      <c r="H1" s="178"/>
     </row>
     <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="48" t="s">
@@ -19263,10 +19502,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="171" t="s">
+      <c r="A3" s="188" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="174" t="s">
+      <c r="B3" s="191" t="s">
         <v>38</v>
       </c>
       <c r="C3" s="143">
@@ -19280,8 +19519,8 @@
       <c r="G3" s="136"/>
     </row>
     <row r="4" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="172"/>
-      <c r="B4" s="151"/>
+      <c r="A4" s="189"/>
+      <c r="B4" s="168"/>
       <c r="C4" s="129">
         <v>2</v>
       </c>
@@ -19293,12 +19532,12 @@
       <c r="G4" s="131"/>
     </row>
     <row r="5" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="172"/>
-      <c r="B5" s="151"/>
+      <c r="A5" s="189"/>
+      <c r="B5" s="168"/>
       <c r="C5" s="129">
         <v>3</v>
       </c>
-      <c r="D5" s="197" t="s">
+      <c r="D5" s="160" t="s">
         <v>41</v>
       </c>
       <c r="E5" s="130"/>
@@ -19306,12 +19545,12 @@
       <c r="G5" s="131"/>
     </row>
     <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="173"/>
-      <c r="B6" s="175"/>
+      <c r="A6" s="190"/>
+      <c r="B6" s="192"/>
       <c r="C6" s="129">
         <v>4</v>
       </c>
-      <c r="D6" s="197" t="s">
+      <c r="D6" s="160" t="s">
         <v>40</v>
       </c>
       <c r="E6" s="130"/>
@@ -19348,8 +19587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19387,48 +19626,48 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="177">
+      <c r="A3" s="195">
         <v>1</v>
       </c>
-      <c r="B3" s="194" t="s">
+      <c r="B3" s="157" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="195" t="s">
+      <c r="C3" s="158" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="195" t="s">
+      <c r="D3" s="158" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="195" t="s">
+      <c r="E3" s="158" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="196" t="s">
+      <c r="F3" s="159" t="s">
         <v>76</v>
       </c>
-      <c r="G3" s="181"/>
+      <c r="G3" s="146"/>
     </row>
     <row r="4" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="177"/>
-      <c r="B4" s="185" t="s">
+      <c r="A4" s="195"/>
+      <c r="B4" s="148" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="179" t="s">
+      <c r="C4" s="144" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="179" t="s">
+      <c r="D4" s="144" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="179" t="s">
+      <c r="E4" s="144" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="186" t="s">
+      <c r="F4" s="149" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="180"/>
+      <c r="G4" s="145"/>
     </row>
     <row r="5" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="177"/>
-      <c r="B5" s="187" t="s">
+      <c r="A5" s="195"/>
+      <c r="B5" s="150" t="s">
         <v>94</v>
       </c>
       <c r="C5" s="139" t="s">
@@ -19440,14 +19679,14 @@
       <c r="E5" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="188" t="s">
+      <c r="F5" s="151" t="s">
         <v>76</v>
       </c>
       <c r="G5" s="141"/>
     </row>
     <row r="6" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="178"/>
-      <c r="B6" s="187" t="s">
+      <c r="A6" s="196"/>
+      <c r="B6" s="150" t="s">
         <v>95</v>
       </c>
       <c r="C6" s="139" t="s">
@@ -19459,16 +19698,16 @@
       <c r="E6" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="188" t="s">
+      <c r="F6" s="151" t="s">
         <v>76</v>
       </c>
       <c r="G6" s="141"/>
     </row>
     <row r="7" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="182">
+      <c r="A7" s="193">
         <v>2</v>
       </c>
-      <c r="B7" s="189" t="s">
+      <c r="B7" s="152" t="s">
         <v>80</v>
       </c>
       <c r="C7" s="139" t="s">
@@ -19480,14 +19719,14 @@
       <c r="E7" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="190" t="s">
+      <c r="F7" s="153" t="s">
         <v>76</v>
       </c>
       <c r="G7" s="140"/>
     </row>
     <row r="8" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="183"/>
-      <c r="B8" s="187" t="s">
+      <c r="A8" s="194"/>
+      <c r="B8" s="150" t="s">
         <v>81</v>
       </c>
       <c r="C8" s="139" t="s">
@@ -19499,14 +19738,14 @@
       <c r="E8" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="188" t="s">
+      <c r="F8" s="151" t="s">
         <v>76</v>
       </c>
       <c r="G8" s="141"/>
     </row>
     <row r="9" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="183"/>
-      <c r="B9" s="187" t="s">
+      <c r="A9" s="194"/>
+      <c r="B9" s="150" t="s">
         <v>82</v>
       </c>
       <c r="C9" s="139" t="s">
@@ -19518,16 +19757,16 @@
       <c r="E9" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="188" t="s">
+      <c r="F9" s="151" t="s">
         <v>76</v>
       </c>
       <c r="G9" s="141"/>
     </row>
     <row r="10" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="182">
+      <c r="A10" s="193">
         <v>3</v>
       </c>
-      <c r="B10" s="189" t="s">
+      <c r="B10" s="152" t="s">
         <v>83</v>
       </c>
       <c r="C10" s="139" t="s">
@@ -19539,14 +19778,14 @@
       <c r="E10" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="190" t="s">
+      <c r="F10" s="153" t="s">
         <v>76</v>
       </c>
       <c r="G10" s="140"/>
     </row>
     <row r="11" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="183"/>
-      <c r="B11" s="187" t="s">
+      <c r="A11" s="194"/>
+      <c r="B11" s="150" t="s">
         <v>84</v>
       </c>
       <c r="C11" s="139" t="s">
@@ -19558,14 +19797,14 @@
       <c r="E11" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="188" t="s">
+      <c r="F11" s="151" t="s">
         <v>76</v>
       </c>
       <c r="G11" s="141"/>
     </row>
     <row r="12" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="183"/>
-      <c r="B12" s="187" t="s">
+      <c r="A12" s="194"/>
+      <c r="B12" s="150" t="s">
         <v>85</v>
       </c>
       <c r="C12" s="139" t="s">
@@ -19577,14 +19816,14 @@
       <c r="E12" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="188" t="s">
+      <c r="F12" s="151" t="s">
         <v>76</v>
       </c>
       <c r="G12" s="141"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="183"/>
-      <c r="B13" s="187" t="s">
+      <c r="A13" s="194"/>
+      <c r="B13" s="150" t="s">
         <v>86</v>
       </c>
       <c r="C13" s="139" t="s">
@@ -19596,16 +19835,16 @@
       <c r="E13" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="188" t="s">
+      <c r="F13" s="151" t="s">
         <v>76</v>
       </c>
       <c r="G13" s="141"/>
     </row>
     <row r="14" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="182">
+      <c r="A14" s="193">
         <v>4</v>
       </c>
-      <c r="B14" s="189" t="s">
+      <c r="B14" s="152" t="s">
         <v>87</v>
       </c>
       <c r="C14" s="139" t="s">
@@ -19617,14 +19856,14 @@
       <c r="E14" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="190" t="s">
+      <c r="F14" s="153" t="s">
         <v>76</v>
       </c>
       <c r="G14" s="140"/>
     </row>
     <row r="15" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="183"/>
-      <c r="B15" s="187" t="s">
+      <c r="A15" s="194"/>
+      <c r="B15" s="150" t="s">
         <v>88</v>
       </c>
       <c r="C15" s="139" t="s">
@@ -19636,14 +19875,14 @@
       <c r="E15" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="188" t="s">
+      <c r="F15" s="151" t="s">
         <v>76</v>
       </c>
       <c r="G15" s="141"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="183"/>
-      <c r="B16" s="187" t="s">
+      <c r="A16" s="194"/>
+      <c r="B16" s="150" t="s">
         <v>89</v>
       </c>
       <c r="C16" s="139" t="s">
@@ -19655,14 +19894,14 @@
       <c r="E16" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="188" t="s">
+      <c r="F16" s="151" t="s">
         <v>76</v>
       </c>
       <c r="G16" s="141"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="183"/>
-      <c r="B17" s="187" t="s">
+      <c r="A17" s="194"/>
+      <c r="B17" s="150" t="s">
         <v>90</v>
       </c>
       <c r="C17" s="139" t="s">
@@ -19674,16 +19913,16 @@
       <c r="E17" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="188" t="s">
+      <c r="F17" s="151" t="s">
         <v>76</v>
       </c>
       <c r="G17" s="141"/>
     </row>
     <row r="18" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="182">
+      <c r="A18" s="193">
         <v>5</v>
       </c>
-      <c r="B18" s="189" t="s">
+      <c r="B18" s="152" t="s">
         <v>91</v>
       </c>
       <c r="C18" s="139" t="s">
@@ -19695,14 +19934,14 @@
       <c r="E18" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="190" t="s">
+      <c r="F18" s="153" t="s">
         <v>76</v>
       </c>
       <c r="G18" s="140"/>
     </row>
     <row r="19" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="183"/>
-      <c r="B19" s="187" t="s">
+      <c r="A19" s="194"/>
+      <c r="B19" s="150" t="s">
         <v>92</v>
       </c>
       <c r="C19" s="139" t="s">
@@ -19714,37 +19953,37 @@
       <c r="E19" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="188" t="s">
+      <c r="F19" s="151" t="s">
         <v>76</v>
       </c>
       <c r="G19" s="141"/>
     </row>
     <row r="20" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="183"/>
-      <c r="B20" s="191" t="s">
+      <c r="A20" s="194"/>
+      <c r="B20" s="154" t="s">
         <v>93</v>
       </c>
-      <c r="C20" s="192" t="s">
+      <c r="C20" s="155" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="192" t="s">
+      <c r="D20" s="155" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="192" t="s">
+      <c r="E20" s="155" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="193" t="s">
+      <c r="F20" s="156" t="s">
         <v>76</v>
       </c>
       <c r="G20" s="141"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="135"/>
-      <c r="B21" s="184"/>
-      <c r="C21" s="184"/>
-      <c r="D21" s="184"/>
-      <c r="E21" s="184"/>
-      <c r="F21" s="184"/>
+      <c r="B21" s="147"/>
+      <c r="C21" s="147"/>
+      <c r="D21" s="147"/>
+      <c r="E21" s="147"/>
+      <c r="F21" s="147"/>
       <c r="G21" s="135"/>
     </row>
   </sheetData>
@@ -19762,25 +20001,416 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="4.140625" customWidth="1"/>
+    <col min="4" max="4" width="40.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="178" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="178"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
+      <c r="H1" s="178"/>
+    </row>
+    <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="207" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="168" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="203">
+        <v>1</v>
+      </c>
+      <c r="D3" s="206" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="204"/>
+      <c r="F3" s="202"/>
+      <c r="G3" s="205"/>
+    </row>
+    <row r="4" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="207"/>
+      <c r="B4" s="168"/>
+      <c r="C4" s="143">
+        <v>2</v>
+      </c>
+      <c r="D4" s="142" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="137"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="136"/>
+    </row>
+    <row r="5" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="207"/>
+      <c r="B5" s="168"/>
+      <c r="C5" s="129">
+        <v>3</v>
+      </c>
+      <c r="D5" s="134" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="130"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
+    </row>
+    <row r="6" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="207"/>
+      <c r="B6" s="168"/>
+      <c r="C6" s="129">
+        <v>4</v>
+      </c>
+      <c r="D6" s="160" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="130"/>
+      <c r="F6" s="131"/>
+      <c r="G6" s="131"/>
+    </row>
+    <row r="7" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="208"/>
+      <c r="B7" s="198"/>
+      <c r="C7" s="129">
+        <v>5</v>
+      </c>
+      <c r="D7" s="160" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="130"/>
+      <c r="F7" s="131"/>
+      <c r="G7" s="131"/>
+    </row>
+    <row r="8" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="131"/>
+      <c r="B8" s="128"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="127"/>
+      <c r="E8" s="130"/>
+      <c r="F8" s="131"/>
+      <c r="G8" s="131"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="A3:A7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="95" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="138" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="61.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="195">
+        <v>1</v>
+      </c>
+      <c r="B2" s="211" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="215"/>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="A3" s="195"/>
+      <c r="B3" s="209" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="212"/>
+      <c r="D3" s="212"/>
+      <c r="E3" s="212"/>
+      <c r="F3" s="212" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="214"/>
+    </row>
+    <row r="4" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="195"/>
+      <c r="B4" s="209" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="212"/>
+      <c r="D4" s="212"/>
+      <c r="E4" s="212"/>
+      <c r="F4" s="212" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="214"/>
+    </row>
+    <row r="5" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="193">
+        <v>2</v>
+      </c>
+      <c r="B5" s="211" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="219"/>
+      <c r="D5" s="219"/>
+      <c r="E5" s="219"/>
+      <c r="F5" s="219" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" s="220"/>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="A6" s="194"/>
+      <c r="B6" s="209" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="212"/>
+      <c r="D6" s="212"/>
+      <c r="E6" s="212"/>
+      <c r="F6" s="212" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" s="214"/>
+    </row>
+    <row r="7" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="194"/>
+      <c r="B7" s="213" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="212"/>
+      <c r="D7" s="212"/>
+      <c r="E7" s="212"/>
+      <c r="F7" s="212" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="214"/>
+    </row>
+    <row r="8" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="193">
+        <v>3</v>
+      </c>
+      <c r="B8" s="221" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="219"/>
+      <c r="D8" s="219"/>
+      <c r="E8" s="219"/>
+      <c r="F8" s="219" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="220"/>
+    </row>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="A9" s="194"/>
+      <c r="B9" s="213" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="212"/>
+      <c r="D9" s="212"/>
+      <c r="E9" s="212"/>
+      <c r="F9" s="212" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" s="214"/>
+    </row>
+    <row r="10" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="194"/>
+      <c r="B10" s="213" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="212"/>
+      <c r="D10" s="212"/>
+      <c r="E10" s="212"/>
+      <c r="F10" s="212" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" s="214"/>
+    </row>
+    <row r="11" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="193">
+        <v>4</v>
+      </c>
+      <c r="B11" s="221" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="219"/>
+      <c r="D11" s="219"/>
+      <c r="E11" s="219"/>
+      <c r="F11" s="219" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="220"/>
+    </row>
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="A12" s="194"/>
+      <c r="B12" s="213" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="212"/>
+      <c r="D12" s="212"/>
+      <c r="E12" s="212"/>
+      <c r="F12" s="212" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="214"/>
+    </row>
+    <row r="13" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="194"/>
+      <c r="B13" s="213" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="212"/>
+      <c r="D13" s="212"/>
+      <c r="E13" s="212"/>
+      <c r="F13" s="212" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="214"/>
+    </row>
+    <row r="14" spans="1:7" ht="60.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="193">
+        <v>5</v>
+      </c>
+      <c r="B14" s="221" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="219"/>
+      <c r="D14" s="219"/>
+      <c r="E14" s="219"/>
+      <c r="F14" s="219" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" s="220"/>
+    </row>
+    <row r="15" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="194"/>
+      <c r="B15" s="222" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="212"/>
+      <c r="D15" s="212"/>
+      <c r="E15" s="212"/>
+      <c r="F15" s="212" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" s="214"/>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="A16" s="194"/>
+      <c r="B16" s="213" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="212"/>
+      <c r="D16" s="212"/>
+      <c r="E16" s="212"/>
+      <c r="F16" s="212" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="214"/>
+    </row>
+    <row r="17" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="194"/>
+      <c r="B17" s="217" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="218"/>
+      <c r="D17" s="218"/>
+      <c r="E17" s="218"/>
+      <c r="F17" s="218" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="216"/>
+    </row>
+    <row r="18" spans="1:7" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B26" s="147"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>